<commit_message>
[1523 zvnl] add to git
</commit_message>
<xml_diff>
--- a/zwnl-9697.xlsx
+++ b/zwnl-9697.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4433FEE6-008E-4E42-BBB7-009B786BB014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75767EC9-16F4-4685-A050-2AE0A21FFFCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7515" yWindow="4118" windowWidth="15247" windowHeight="11647" xr2:uid="{D33B17E7-9394-4FC9-A188-FF576B280660}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{D33B17E7-9394-4FC9-A188-FF576B280660}"/>
   </bookViews>
   <sheets>
     <sheet name="Spotten" sheetId="1" r:id="rId1"/>
@@ -40,6 +40,30 @@
     <author>Tom</author>
   </authors>
   <commentList>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{9E46BBB8-0AC7-42E9-9C51-7DE9410B7726}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Speler rood sein inrijder Rsd</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B4" authorId="0" shapeId="0" xr:uid="{1F4111D6-9AB0-4662-90A1-B73A15D4FE18}">
       <text>
         <r>
@@ -69,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Naam</t>
   </si>
@@ -764,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F8B9C10-3B26-4BBA-B6EF-00E5872C35E1}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -802,7 +826,7 @@
       <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -922,6 +946,9 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>